<commit_message>
Generar reporte en formato Excel parte2
</commit_message>
<xml_diff>
--- a/Excel/reporte_productos.xlsx
+++ b/Excel/reporte_productos.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>Reporte de productos en Excel</t>
   </si>
@@ -45,6 +45,51 @@
   </si>
   <si>
     <t>precio</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>0.5 mg</t>
+  </si>
+  <si>
+    <t>Cajita</t>
+  </si>
+  <si>
+    <t>Amount1</t>
+  </si>
+  <si>
+    <t>Crema</t>
+  </si>
+  <si>
+    <t>comerciales</t>
+  </si>
+  <si>
+    <t>Baselina</t>
+  </si>
+  <si>
+    <t>600 mg</t>
+  </si>
+  <si>
+    <t>Caja vial</t>
+  </si>
+  <si>
+    <t>Novartis</t>
+  </si>
+  <si>
+    <t>Sobresitos</t>
+  </si>
+  <si>
+    <t>Mentisan</t>
+  </si>
+  <si>
+    <t>500gr.</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Inti</t>
   </si>
 </sst>
 </file>
@@ -52,7 +97,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -80,6 +125,15 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -104,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -112,6 +166,9 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -413,13 +470,23 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A4" sqref="A4:I4"/>
+      <selection activeCell="A5" sqref="A5:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="16" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="13" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="15" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="13" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="6" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="8" bestFit="true" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
@@ -453,6 +520,91 @@
       </c>
       <c r="I4" s="2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6">
+        <v>132</v>
+      </c>
+      <c r="I6">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>86</v>
+      </c>
+      <c r="I7">
+        <v>7.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion de modulo gestion lote parte 10
</commit_message>
<xml_diff>
--- a/Excel/reporte_productos.xlsx
+++ b/Excel/reporte_productos.xlsx
@@ -97,7 +97,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -125,15 +125,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -158,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -166,9 +157,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -473,7 +461,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A5" sqref="A5:I5"/>
+      <selection activeCell="A4" sqref="A4:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -523,29 +511,31 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="3">
+      <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3">
+      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="I5">
         <v>1.2</v>
       </c>
     </row>
@@ -572,7 +562,7 @@
         <v>20</v>
       </c>
       <c r="H6">
-        <v>132</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <v>2.7</v>
@@ -601,10 +591,10 @@
         <v>15</v>
       </c>
       <c r="H7">
-        <v>86</v>
+        <v>4</v>
       </c>
       <c r="I7">
-        <v>7.5</v>
+        <v>7.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>